<commit_message>
Refined Table structure für database
</commit_message>
<xml_diff>
--- a/P2 - DB.xlsx
+++ b/P2 - DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_P2\cms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066D960D-4732-4838-B9FF-8DEAF6FA07F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74033270-15A6-478D-953C-456FAE889B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,9 +196,6 @@
     <t>Rotation</t>
   </si>
   <si>
-    <t>(FK) Scene</t>
-  </si>
-  <si>
     <t>(FK) Asset Type</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>(Asset deleted? -&gt; True ==&gt; Purge Database in regular intervals)</t>
+  </si>
+  <si>
+    <t>(FK) SceneID</t>
   </si>
 </sst>
 </file>
@@ -325,11 +325,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED9476B-7BB8-4342-83E8-55315D79D9E7}">
   <dimension ref="B2:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,21 +663,21 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C5" t="s">
@@ -715,7 +715,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C10" t="s">
@@ -742,8 +742,8 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>61</v>
+      <c r="B14" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
@@ -797,29 +797,29 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
         <v>68</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>75</v>
       </c>
-      <c r="E21" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>62</v>
+      <c r="B23" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
@@ -836,31 +836,31 @@
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>66</v>
+      <c r="B28" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
@@ -885,12 +885,12 @@
         <v>27</v>
       </c>
       <c r="E30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -901,13 +901,13 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
         <v>72</v>
-      </c>
-      <c r="D33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -919,7 +919,7 @@
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C36" t="s">
@@ -938,7 +938,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C39" t="s">
@@ -950,7 +950,7 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
         <v>43</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D42" t="s">
         <v>43</v>
@@ -980,7 +980,7 @@
         <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>27</v>
       </c>
       <c r="E44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
         <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1025,18 +1025,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Finalized Database Layout. Included SQL creation script
</commit_message>
<xml_diff>
--- a/P2 - DB.xlsx
+++ b/P2 - DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_P2\cms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74033270-15A6-478D-953C-456FAE889B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC67287-BB3D-4EDD-9E1F-3042883E90AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t>P2 - Datenbank Layout</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Keys</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>Surname</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>(FK) Creator</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>Scene</t>
   </si>
   <si>
@@ -196,12 +190,6 @@
     <t>Rotation</t>
   </si>
   <si>
-    <t>(FK) Asset Type</t>
-  </si>
-  <si>
-    <t>(FK) Asset ID</t>
-  </si>
-  <si>
     <t>(will be Vec3 as string -&gt; parse as you go)</t>
   </si>
   <si>
@@ -238,15 +226,6 @@
     <t>(Similar to SceneAsset)</t>
   </si>
   <si>
-    <t>AssetType</t>
-  </si>
-  <si>
-    <t>Designator</t>
-  </si>
-  <si>
-    <t>(3DModel, Light, Marker)</t>
-  </si>
-  <si>
     <t>Deleted</t>
   </si>
   <si>
@@ -256,7 +235,40 @@
     <t>(Asset deleted? -&gt; True ==&gt; Purge Database in regular intervals)</t>
   </si>
   <si>
-    <t>(FK) SceneID</t>
+    <t>SceneAssetAnchor</t>
+  </si>
+  <si>
+    <t>LightAnchor</t>
+  </si>
+  <si>
+    <t>MarkerAnchor</t>
+  </si>
+  <si>
+    <t>AnchorID</t>
+  </si>
+  <si>
+    <t>SceneID</t>
+  </si>
+  <si>
+    <t>AssetID</t>
+  </si>
+  <si>
+    <t>*Shared Primary Key and Class Table Inheritance</t>
+  </si>
+  <si>
+    <t>CourseID</t>
+  </si>
+  <si>
+    <t>CreatorID</t>
+  </si>
+  <si>
+    <t>LightAsset Table</t>
+  </si>
+  <si>
+    <t>MarkerAssetTable</t>
+  </si>
+  <si>
+    <t>SceneAssetTable</t>
   </si>
 </sst>
 </file>
@@ -288,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -321,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -330,6 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -645,15 +664,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED9476B-7BB8-4342-83E8-55315D79D9E7}">
-  <dimension ref="B2:E45"/>
+  <dimension ref="B2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -670,29 +689,29 @@
         <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -700,7 +719,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -708,7 +727,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -716,18 +735,18 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -735,7 +754,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
@@ -743,29 +762,29 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -781,228 +800,259 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
         <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
       </c>
-      <c r="E21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>42</v>
-      </c>
       <c r="D24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
         <v>62</v>
-      </c>
-      <c r="D25" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>43</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="C48" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" t="s">
-        <v>58</v>
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>